<commit_message>
Works better with outside directories, more tests
</commit_message>
<xml_diff>
--- a/testFiles/smart_toilet_test2/smart_toilet2_lengths.xlsx
+++ b/testFiles/smart_toilet_test2/smart_toilet2_lengths.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">wire</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">soln3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connect1_1</t>
   </si>
 </sst>
 </file>
@@ -175,17 +178,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -283,10 +286,18 @@
         <v>0.01</v>
       </c>
     </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>